<commit_message>
VTable only size N + multiCompeteOthello
several smaller SW changes
- in many agent files: ensure that getNextAction2 returns an ACTIONS_VT object having a vTable with exactly N = so.availableActions.size() elements (and not N+1)
- simplified moveProbabilitiesFor VTable accordingly
- multiCompeteOthello results
- AgentBase.setWrapperParams: to save all actual wrapper params
- parameter largestDepth in MCTSWrapper
- bug fix Arena.InspectGame: ConfigWrapper.USELASTMCTS has to be false during InspectGame
- extended MCompeteOthello for potential c_puct sweep
- made one constructor of Types.ACTIONS_VT obsolete
</commit_message>
<xml_diff>
--- a/agents/Othello/csv/multiCompeteOthello-i10000.xlsx
+++ b/agents/Othello/csv/multiCompeteOthello-i10000.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfgang\Documents\GitHub\GBG\agents\Othello\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01CFCF64-941C-4A8C-9433-853153B125D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BAC89D-E33F-4BB6-8036-AB21070D5DB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8592"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="multiCompeteOthello-i10000" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'multiCompeteOthello-i10000'!$A$3:$J$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'multiCompeteOthello-i10000'!$A$3:$J$57</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -65,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -900,27 +899,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4:H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <f>SUBTOTAL(1,H4:H57)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -952,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -984,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1016,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1080,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1112,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1144,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1176,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1208,7 +1212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1240,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1272,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1304,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1336,7 +1340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -1400,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1432,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1464,7 +1468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1496,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1592,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
@@ -1624,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
@@ -1656,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -1688,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1784,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0</v>
       </c>
@@ -1816,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1848,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
@@ -1880,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
@@ -1976,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0</v>
       </c>
@@ -2008,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0</v>
       </c>
@@ -2040,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
@@ -2072,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0</v>
       </c>
@@ -2200,7 +2204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
@@ -2232,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>0</v>
       </c>
@@ -2264,7 +2268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>0</v>
       </c>
@@ -2360,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0</v>
       </c>
@@ -2392,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
@@ -2424,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>0</v>
       </c>
@@ -2456,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>0</v>
       </c>
@@ -2552,7 +2556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>0</v>
       </c>
@@ -2584,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>0</v>
       </c>
@@ -2616,7 +2620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0</v>
       </c>
@@ -2648,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>0</v>
       </c>
@@ -2681,7 +2685,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:J3"/>
+  <autoFilter ref="A3:J57" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1.00E-08"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>